<commit_message>
Added datasheets and spreadsheets for calculations:
</commit_message>
<xml_diff>
--- a/Datasheets/SpecificationCalculations.xlsx
+++ b/Datasheets/SpecificationCalculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonhu\Documents\UBC 2018\ELEC 491\Github\SolarFlorez\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6085C67-57FD-4CCD-83C1-A3E48B9D5C9E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560C13B4-E9AA-4AF7-A6EE-286D1CDF0D7B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="8112" xr2:uid="{7E0B657F-185B-46C3-9CE5-F8FC01038B87}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Boost MOSFET Specifications</t>
   </si>
@@ -96,12 +96,6 @@
     <t>Selected</t>
   </si>
   <si>
-    <t>1727-2591-1-ND</t>
-  </si>
-  <si>
-    <t>PSMN015-100YLX</t>
-  </si>
-  <si>
     <t>Cont Max Vds</t>
   </si>
   <si>
@@ -124,6 +118,9 @@
   </si>
   <si>
     <t>Vf</t>
+  </si>
+  <si>
+    <t>IPP114N12N3GXKSA1-ND</t>
   </si>
 </sst>
 </file>
@@ -161,11 +158,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +480,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -493,11 +490,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -506,10 +503,10 @@
       <c r="B2">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -518,10 +515,10 @@
       <c r="B3">
         <v>242</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1"/>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -530,10 +527,8 @@
       <c r="B4">
         <v>16.420000000000002</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -569,23 +564,23 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.4999999999999999E-2</v>
+        <v>1.14E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>3.2000000000000002E-8</v>
+      <c r="B10" s="1">
+        <v>3.5999999999999998E-8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>5.8999999999999999E-8</v>
+      <c r="B11" s="1">
+        <v>6.9999999999999998E-9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -599,25 +594,25 @@
       </c>
       <c r="B13">
         <f>B4*B4*B9</f>
-        <v>4.0442460000000011</v>
+        <v>3.0736269600000008</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <f>0.5*B4*B7*(B10+B11)*B17</f>
-        <v>1.8895487738400005</v>
+        <v>0.89286370632000023</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <f>0.5*B4*B7*(B10+B11)*B17</f>
-        <v>1.8895487738400005</v>
+        <v>0.89286370632000023</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -626,7 +621,7 @@
       </c>
       <c r="B16">
         <f>SUM(B13:B15)</f>
-        <v>7.8233435476800022</v>
+        <v>4.8593543726400013</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -651,18 +646,18 @@
       </c>
       <c r="B19">
         <f>B16*B18</f>
-        <v>6.023974531713602</v>
+        <v>3.7417028669328012</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="D21" s="1" t="s">
+      <c r="B21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
@@ -671,10 +666,10 @@
       <c r="B22">
         <v>116</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="1"/>
+      <c r="D22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
@@ -683,10 +678,8 @@
       <c r="B23">
         <v>445</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="1"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
@@ -714,7 +707,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B27">
         <v>73</v>
@@ -730,23 +723,23 @@
         <v>8</v>
       </c>
       <c r="B29">
-        <v>1.4999999999999999E-2</v>
+        <v>1.14E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="2">
-        <v>3.2000000000000002E-8</v>
+      <c r="B30" s="1">
+        <v>3.5999999999999998E-8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="2">
-        <v>5.8999999999999999E-8</v>
+      <c r="B31" s="1">
+        <v>6.9999999999999998E-9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -760,25 +753,25 @@
       </c>
       <c r="B33">
         <f>B24*B24*B29</f>
-        <v>13.186837499999999</v>
+        <v>10.0219965</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <f>0.5*B27*B24*(B30+B31)*B37</f>
-        <v>2.2650969249999999</v>
+        <v>1.0703205250000001</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <f>B34</f>
-        <v>2.2650969249999999</v>
+        <v>1.0703205250000001</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -787,7 +780,7 @@
       </c>
       <c r="B36">
         <f>SUM(B33:B35)</f>
-        <v>17.717031349999999</v>
+        <v>12.162637549999999</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -812,7 +805,7 @@
       </c>
       <c r="B39">
         <f>B38*B36</f>
-        <v>13.6421141395</v>
+        <v>9.3652309134999996</v>
       </c>
     </row>
   </sheetData>
@@ -845,22 +838,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>112</v>
@@ -868,7 +861,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -876,7 +869,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0.7</v>
@@ -892,14 +885,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>147.5</v>
@@ -907,7 +900,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>56</v>
@@ -915,7 +908,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>0.7</v>

</xml_diff>

<commit_message>
Edits made during key documents generation
</commit_message>
<xml_diff>
--- a/Datasheets/SpecificationCalculations.xlsx
+++ b/Datasheets/SpecificationCalculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonhu\Documents\UBC 2018\ELEC 491\Github\SolarFlorez\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560C13B4-E9AA-4AF7-A6EE-286D1CDF0D7B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D3A4E5-4719-4ABB-811B-D53D16AEAEDD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="8112" xr2:uid="{7E0B657F-185B-46C3-9CE5-F8FC01038B87}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MOSFETs" sheetId="1" r:id="rId1"/>
     <sheet name="Diodes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>Boost MOSFET Specifications</t>
   </si>
@@ -121,6 +122,12 @@
   </si>
   <si>
     <t>IPP114N12N3GXKSA1-ND</t>
+  </si>
+  <si>
+    <t>R Junction Case</t>
+  </si>
+  <si>
+    <t>Buck MOSFET Specifications - Low Side</t>
   </si>
 </sst>
 </file>
@@ -144,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,14 +159,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,24 +500,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952B0972-9DAB-48EC-9F90-6207E69AA8E7}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.83984375" customWidth="1"/>
+    <col min="1" max="1" width="21.1015625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1015625" customWidth="1"/>
+    <col min="5" max="5" width="16.3125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -503,10 +527,10 @@
       <c r="B2">
         <v>34</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -515,10 +539,10 @@
       <c r="B3">
         <v>242</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -527,8 +551,8 @@
       <c r="B4">
         <v>16.420000000000002</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -560,7 +584,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -568,7 +592,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -576,7 +600,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -584,12 +608,12 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B13">
@@ -598,7 +622,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2">
@@ -607,7 +631,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1">
@@ -616,7 +640,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16">
@@ -625,7 +649,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17">
@@ -633,31 +657,31 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>18</v>
+      <c r="A18" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B18">
-        <v>0.77</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <f>B16*B18</f>
-        <v>3.7417028669328012</v>
+        <v>5.3452898099040018</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="D21" s="3" t="s">
+      <c r="B21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
@@ -666,10 +690,10 @@
       <c r="B22">
         <v>116</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
@@ -678,8 +702,8 @@
       <c r="B23">
         <v>445</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
@@ -796,7 +820,7 @@
         <v>18</v>
       </c>
       <c r="B38">
-        <v>0.77</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -805,11 +829,161 @@
       </c>
       <c r="B39">
         <f>B38*B36</f>
-        <v>9.3652309134999996</v>
+        <v>13.378901305000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>11.13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>112.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49">
+        <v>3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5.8999999999999999E-8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.4E-8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <f>B44*B44*B49</f>
+        <v>19.11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="1">
+        <f>0.5*B47*B44*(B50+B51)*B57</f>
+        <v>4.2898450000000006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="1">
+        <f>B54</f>
+        <v>4.2898450000000006</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56">
+        <f>SUM(B53:B55)</f>
+        <v>27.689689999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59">
+        <f>B58*B56</f>
+        <v>19.382782999999996</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="A1:C1"/>
@@ -829,7 +1003,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -838,18 +1012,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -885,10 +1059,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">

</xml_diff>